<commit_message>
commit@20220327 fix 错料 issue.
</commit_message>
<xml_diff>
--- a/[HW]my_heat/my_heat bom.xlsx
+++ b/[HW]my_heat/my_heat bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\my_heat\[HW]my_heat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055FE370-8267-4C09-8AEE-B2DA6BAEB6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB9AA1E-9F64-4609-89F3-A1B1F65E7391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="739" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="253">
   <si>
     <r>
       <rPr>
@@ -374,9 +374,6 @@
   </si>
   <si>
     <t>安装方式SMD,阻值12K,精度±1%,0603,额定功率1/10W</t>
-  </si>
-  <si>
-    <t>SIQ-02FVS3</t>
   </si>
   <si>
     <t>IC THERMOCOUP TO DGTL 8-SOIC</t>
@@ -922,14 +919,6 @@
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
   <si>
-    <t>KH-DC-007B-2.1G</t>
-    <phoneticPr fontId="26" type="noConversion"/>
-  </si>
-  <si>
-    <t>错料</t>
-    <phoneticPr fontId="26" type="noConversion"/>
-  </si>
-  <si>
     <t>K5-1672SN-01</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
@@ -974,6 +963,16 @@
   </si>
   <si>
     <t xml:space="preserve">YAGEO, YAGEO, YAGEO, YAGEO, YAGEO, YAGEO, YAGEO, YAGEO, YAGEO, , YAGEO, YAGEO, YAGEO, YAGEO, </t>
+  </si>
+  <si>
+    <t>'SIQ-02FVS3</t>
+  </si>
+  <si>
+    <t>KH-DC-007B-2.5G</t>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="26" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1181,13 +1180,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="宋体"/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1209,12 +1208,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1381,7 +1374,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1492,33 +1485,65 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="19"/>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1526,9 +1551,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1540,39 +1562,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="3级" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2429,8 +2419,8 @@
   </sheetPr>
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -2457,117 +2447,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
       <c r="Q1" s="15"/>
     </row>
     <row r="2" spans="2:19" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
       <c r="Q2" s="16"/>
     </row>
     <row r="3" spans="2:19" s="3" customFormat="1" ht="57" customHeight="1">
-      <c r="B3" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54" t="s">
+      <c r="B3" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="55" t="s">
+      <c r="H3" s="63"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="56"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
       <c r="Q3" s="17"/>
     </row>
     <row r="4" spans="2:19" s="3" customFormat="1" ht="35.25" customHeight="1">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53" t="s">
+      <c r="C4" s="51"/>
+      <c r="D4" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="58" t="s">
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58" t="s">
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
       <c r="Q4" s="18"/>
     </row>
     <row r="5" spans="2:19" s="4" customFormat="1" ht="35.25" customHeight="1">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="60"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="58"/>
       <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="2:19" s="4" customFormat="1" ht="42.75" customHeight="1">
@@ -2586,11 +2576,11 @@
       <c r="F6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="6" t="s">
         <v>18</v>
       </c>
@@ -2628,29 +2618,29 @@
       <c r="F7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="63" t="s">
+      <c r="G7" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="65"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M7" s="23"/>
       <c r="N7" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O7" s="23"/>
       <c r="P7" s="24"/>
       <c r="Q7" s="29"/>
       <c r="S7" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" customHeight="1">
@@ -2665,28 +2655,28 @@
       <c r="F8" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
       <c r="J8" s="34" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L8" s="10">
         <v>8</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O8" s="13"/>
       <c r="P8" s="14"/>
       <c r="S8" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.75" customHeight="1">
@@ -2701,28 +2691,28 @@
       <c r="F9" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="47" t="s">
         <v>73</v>
       </c>
       <c r="H9" s="48"/>
       <c r="I9" s="49"/>
       <c r="J9" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L9" s="10">
         <v>2</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O9" s="13"/>
       <c r="P9" s="14"/>
       <c r="S9" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" customHeight="1">
@@ -2737,28 +2727,28 @@
       <c r="F10" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="G10" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="53"/>
       <c r="J10" s="34" t="s">
         <v>2</v>
       </c>
       <c r="K10" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L10" s="10">
         <v>4</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O10" s="13"/>
       <c r="P10" s="14"/>
       <c r="S10" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="15.75" customHeight="1">
@@ -2773,7 +2763,7 @@
       <c r="F11" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="45" t="s">
+      <c r="G11" s="47" t="s">
         <v>75</v>
       </c>
       <c r="H11" s="48"/>
@@ -2782,19 +2772,19 @@
         <v>2</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L11" s="10">
         <v>2</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O11" s="13"/>
       <c r="P11" s="14"/>
       <c r="S11" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="15.75" customHeight="1">
@@ -2809,28 +2799,28 @@
       <c r="F12" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="53"/>
       <c r="J12" s="34" t="s">
         <v>2</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L12" s="10">
         <v>3</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O12" s="13"/>
       <c r="P12" s="14"/>
       <c r="S12" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="2:19" ht="15.75" customHeight="1">
@@ -2845,28 +2835,28 @@
       <c r="F13" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="47" t="s">
         <v>77</v>
       </c>
       <c r="H13" s="48"/>
       <c r="I13" s="49"/>
       <c r="J13" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K13" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L13" s="10">
         <v>3</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O13" s="13"/>
       <c r="P13" s="14"/>
       <c r="S13" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="15.75" customHeight="1">
@@ -2881,28 +2871,28 @@
       <c r="F14" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="G14" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="46"/>
-      <c r="I14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="53"/>
       <c r="J14" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K14" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L14" s="10">
         <v>1</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O14" s="13"/>
       <c r="P14" s="14"/>
       <c r="S14" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="2:19" ht="15.75" customHeight="1">
@@ -2917,28 +2907,28 @@
       <c r="F15" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G15" s="47" t="s">
         <v>79</v>
       </c>
       <c r="H15" s="48"/>
       <c r="I15" s="49"/>
       <c r="J15" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K15" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L15" s="10">
         <v>3</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O15" s="13"/>
       <c r="P15" s="14"/>
       <c r="S15" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="2:19" ht="15.75" customHeight="1">
@@ -2953,7 +2943,7 @@
       <c r="F16" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="47" t="s">
         <v>88</v>
       </c>
       <c r="H16" s="48"/>
@@ -2962,14 +2952,14 @@
         <v>2</v>
       </c>
       <c r="K16" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L16" s="10">
         <v>3</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O16" s="13"/>
       <c r="P16" s="14"/>
@@ -2989,23 +2979,23 @@
       <c r="F17" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
       <c r="J17" s="34" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K17" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L17" s="10">
         <v>15</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O17" s="13"/>
       <c r="P17" s="14"/>
@@ -3025,7 +3015,7 @@
       <c r="F18" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="47" t="s">
         <v>90</v>
       </c>
       <c r="H18" s="48"/>
@@ -3034,14 +3024,14 @@
         <v>2</v>
       </c>
       <c r="K18" s="35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L18" s="10">
         <v>5</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O18" s="13"/>
       <c r="P18" s="14"/>
@@ -3061,23 +3051,23 @@
       <c r="F19" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="45" t="s">
+      <c r="G19" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="53"/>
       <c r="J19" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K19" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L19" s="10">
         <v>2</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O19" s="13"/>
       <c r="P19" s="14"/>
@@ -3097,7 +3087,7 @@
       <c r="F20" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="47" t="s">
         <v>92</v>
       </c>
       <c r="H20" s="48"/>
@@ -3106,14 +3096,14 @@
         <v>2</v>
       </c>
       <c r="K20" s="35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L20" s="10">
         <v>1</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O20" s="13"/>
       <c r="P20" s="14"/>
@@ -3133,23 +3123,23 @@
       <c r="F21" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="46"/>
-      <c r="I21" s="47"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="53"/>
       <c r="J21" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K21" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L21" s="10">
         <v>2</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O21" s="13"/>
       <c r="P21" s="14"/>
@@ -3169,7 +3159,7 @@
       <c r="F22" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="47" t="s">
         <v>94</v>
       </c>
       <c r="H22" s="48"/>
@@ -3178,14 +3168,14 @@
         <v>2</v>
       </c>
       <c r="K22" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L22" s="10">
         <v>3</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O22" s="13"/>
       <c r="P22" s="14"/>
@@ -3205,28 +3195,28 @@
       <c r="F23" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="H23" s="46"/>
-      <c r="I23" s="47"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="53"/>
       <c r="J23" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K23" s="35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L23" s="10">
         <v>1</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O23" s="13"/>
       <c r="P23" s="14"/>
       <c r="S23" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="2:19" ht="15.75" customHeight="1">
@@ -3241,7 +3231,7 @@
       <c r="F24" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="45" t="s">
+      <c r="G24" s="47" t="s">
         <v>96</v>
       </c>
       <c r="H24" s="48"/>
@@ -3250,14 +3240,14 @@
         <v>2</v>
       </c>
       <c r="K24" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L24" s="10">
         <v>2</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O24" s="13"/>
       <c r="P24" s="14"/>
@@ -3277,23 +3267,23 @@
       <c r="F25" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G25" s="45" t="s">
+      <c r="G25" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="53"/>
       <c r="J25" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K25" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L25" s="10">
         <v>1</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O25" s="13"/>
       <c r="P25" s="14"/>
@@ -3313,23 +3303,23 @@
       <c r="F26" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G26" s="47" t="s">
         <v>98</v>
       </c>
       <c r="H26" s="48"/>
       <c r="I26" s="49"/>
       <c r="J26" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L26" s="10">
         <v>4</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O26" s="13"/>
       <c r="P26" s="14"/>
@@ -3349,23 +3339,23 @@
       <c r="F27" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="45" t="s">
+      <c r="G27" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="H27" s="46"/>
-      <c r="I27" s="47"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="53"/>
       <c r="J27" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K27" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L27" s="10">
         <v>2</v>
       </c>
       <c r="M27" s="10"/>
       <c r="N27" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O27" s="13"/>
       <c r="P27" s="14"/>
@@ -3385,7 +3375,7 @@
       <c r="F28" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G28" s="45" t="s">
+      <c r="G28" s="47" t="s">
         <v>100</v>
       </c>
       <c r="H28" s="48"/>
@@ -3394,14 +3384,14 @@
         <v>2</v>
       </c>
       <c r="K28" s="35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L28" s="10">
         <v>2</v>
       </c>
       <c r="M28" s="10"/>
       <c r="N28" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O28" s="13"/>
       <c r="P28" s="14"/>
@@ -3421,23 +3411,23 @@
       <c r="F29" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="45" t="s">
+      <c r="G29" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="47"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="53"/>
       <c r="J29" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K29" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L29" s="10">
         <v>2</v>
       </c>
       <c r="M29" s="10"/>
       <c r="N29" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O29" s="13"/>
       <c r="P29" s="14"/>
@@ -3457,28 +3447,28 @@
       <c r="F30" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="45" t="s">
+      <c r="G30" s="47" t="s">
         <v>80</v>
       </c>
       <c r="H30" s="48"/>
       <c r="I30" s="49"/>
       <c r="J30" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K30" s="35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L30" s="10">
         <v>1</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O30" s="13"/>
       <c r="P30" s="14"/>
       <c r="S30" s="36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="2:19" ht="15.75" customHeight="1">
@@ -3493,28 +3483,28 @@
       <c r="F31" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="45" t="s">
+      <c r="G31" s="47" t="s">
         <v>85</v>
       </c>
       <c r="H31" s="48"/>
       <c r="I31" s="49"/>
       <c r="J31" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K31" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L31" s="10">
         <v>2</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O31" s="13"/>
       <c r="P31" s="14"/>
       <c r="S31" s="36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="2:19" ht="15.75" customHeight="1">
@@ -3529,28 +3519,28 @@
       <c r="F32" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G32" s="45" t="s">
+      <c r="G32" s="47" t="s">
         <v>86</v>
       </c>
       <c r="H32" s="48"/>
       <c r="I32" s="49"/>
       <c r="J32" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K32" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L32" s="10">
         <v>4</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O32" s="13"/>
       <c r="P32" s="14"/>
       <c r="S32" s="36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="2:19" ht="15.75" customHeight="1">
@@ -3565,28 +3555,28 @@
       <c r="F33" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="47"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="53"/>
       <c r="J33" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K33" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L33" s="10">
         <v>1</v>
       </c>
       <c r="M33" s="10"/>
       <c r="N33" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O33" s="13"/>
       <c r="P33" s="14"/>
       <c r="S33" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="2:19" ht="15.75" customHeight="1">
@@ -3601,8 +3591,8 @@
       <c r="F34" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="50" t="s">
-        <v>221</v>
+      <c r="G34" s="54" t="s">
+        <v>220</v>
       </c>
       <c r="H34" s="48"/>
       <c r="I34" s="49"/>
@@ -3610,17 +3600,17 @@
         <v>2</v>
       </c>
       <c r="K34" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L34" s="10">
         <v>1</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O34" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P34" s="14"/>
       <c r="S34" s="36" t="s">
@@ -3639,32 +3629,32 @@
       <c r="F35" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G35" s="45" t="s">
-        <v>103</v>
+      <c r="G35" s="47" t="s">
+        <v>102</v>
       </c>
       <c r="H35" s="48"/>
       <c r="I35" s="49"/>
       <c r="J35" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K35" s="35" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="L35" s="10">
         <v>1</v>
       </c>
       <c r="M35" s="10"/>
       <c r="N35" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O35" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P35" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P35" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S35" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="2:19" ht="15.75" customHeight="1">
@@ -3679,32 +3669,32 @@
       <c r="F36" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="G36" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="H36" s="46"/>
-      <c r="I36" s="47"/>
+      <c r="G36" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="52"/>
+      <c r="I36" s="53"/>
       <c r="J36" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K36" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L36" s="10">
         <v>1</v>
       </c>
       <c r="M36" s="10"/>
       <c r="N36" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O36" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P36" s="42" t="s">
-        <v>250</v>
+        <v>234</v>
+      </c>
+      <c r="P36" s="41" t="s">
+        <v>247</v>
       </c>
       <c r="S36" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="2:19" ht="15.75" customHeight="1">
@@ -3719,32 +3709,32 @@
       <c r="F37" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G37" s="45" t="s">
+      <c r="G37" s="47" t="s">
         <v>2</v>
       </c>
       <c r="H37" s="48"/>
       <c r="I37" s="49"/>
       <c r="J37" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K37" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L37" s="10">
         <v>1</v>
       </c>
       <c r="M37" s="10"/>
       <c r="N37" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O37" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P37" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P37" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S37" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="2:19" ht="15.75" customHeight="1">
@@ -3759,32 +3749,32 @@
       <c r="F38" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H38" s="46"/>
-      <c r="I38" s="47"/>
+      <c r="G38" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" s="52"/>
+      <c r="I38" s="53"/>
       <c r="J38" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K38" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L38" s="10">
         <v>1</v>
       </c>
       <c r="M38" s="10"/>
       <c r="N38" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O38" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P38" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P38" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S38" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="2:19" ht="15.75" customHeight="1">
@@ -3799,7 +3789,7 @@
       <c r="F39" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G39" s="45" t="s">
+      <c r="G39" s="47" t="s">
         <v>2</v>
       </c>
       <c r="H39" s="48"/>
@@ -3808,23 +3798,23 @@
         <v>2</v>
       </c>
       <c r="K39" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L39" s="10">
         <v>1</v>
       </c>
       <c r="M39" s="10"/>
       <c r="N39" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O39" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P39" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P39" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S39" s="36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="2:19" ht="15.75" customHeight="1">
@@ -3839,38 +3829,36 @@
       <c r="F40" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="H40" s="46"/>
-      <c r="I40" s="47"/>
+      <c r="G40" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="H40" s="52"/>
+      <c r="I40" s="53"/>
       <c r="J40" s="34" t="s">
         <v>2</v>
       </c>
       <c r="K40" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L40" s="10">
         <v>1</v>
       </c>
       <c r="M40" s="10"/>
       <c r="N40" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O40" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P40" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P40" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S40" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B41" s="40" t="s">
-        <v>243</v>
-      </c>
+      <c r="B41" s="7"/>
       <c r="C41" s="8">
         <v>4</v>
       </c>
@@ -3881,32 +3869,32 @@
       <c r="F41" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="50" t="s">
+      <c r="G41" s="54" t="s">
         <v>2</v>
       </c>
       <c r="H41" s="48"/>
       <c r="I41" s="49"/>
       <c r="J41" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K41" s="35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L41" s="10">
         <v>1</v>
       </c>
       <c r="M41" s="10"/>
       <c r="N41" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O41" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P41" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P41" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S41" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="2:19" ht="15.75" customHeight="1">
@@ -3919,33 +3907,33 @@
         <v>2</v>
       </c>
       <c r="F42" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="G42" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="G42" s="50" t="s">
+      <c r="H42" s="52"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="H42" s="46"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="39" t="s">
-        <v>232</v>
-      </c>
-      <c r="K42" s="35"/>
+      <c r="K42" s="35" t="s">
+        <v>250</v>
+      </c>
       <c r="L42" s="10">
         <v>1</v>
       </c>
       <c r="M42" s="10"/>
       <c r="N42" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O42" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P42" s="42" t="s">
-        <v>239</v>
-      </c>
-      <c r="S42" s="36" t="s">
-        <v>102</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="P42" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="S42" s="36"/>
     </row>
     <row r="43" spans="2:19" ht="15.75" customHeight="1">
       <c r="B43" s="7"/>
@@ -3959,30 +3947,32 @@
       <c r="F43" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G43" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H43" s="67"/>
-      <c r="I43" s="68"/>
+      <c r="G43" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="55"/>
+      <c r="I43" s="56"/>
       <c r="J43" s="34" t="s">
         <v>2</v>
       </c>
       <c r="K43" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L43" s="10">
         <v>1</v>
       </c>
       <c r="M43" s="10"/>
       <c r="N43" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O43" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P43" s="44"/>
+        <v>234</v>
+      </c>
+      <c r="P43" s="67" t="s">
+        <v>252</v>
+      </c>
       <c r="S43" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="2:19" ht="15.75" customHeight="1">
@@ -3997,32 +3987,32 @@
       <c r="F44" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G44" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H44" s="46"/>
-      <c r="I44" s="47"/>
+      <c r="G44" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H44" s="52"/>
+      <c r="I44" s="53"/>
       <c r="J44" s="34" t="s">
         <v>2</v>
       </c>
       <c r="K44" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L44" s="10">
         <v>1</v>
       </c>
       <c r="M44" s="10"/>
       <c r="N44" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="O44" s="43" t="s">
-        <v>247</v>
-      </c>
-      <c r="P44" s="42" t="s">
-        <v>239</v>
+        <v>157</v>
+      </c>
+      <c r="O44" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="P44" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S44" s="36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="2:19" ht="15.75" customHeight="1">
@@ -4037,32 +4027,32 @@
       <c r="F45" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G45" s="45" t="s">
+      <c r="G45" s="47" t="s">
         <v>2</v>
       </c>
       <c r="H45" s="48"/>
       <c r="I45" s="49"/>
       <c r="J45" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K45" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L45" s="10">
         <v>1</v>
       </c>
       <c r="M45" s="10"/>
       <c r="N45" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O45" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P45" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P45" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S45" s="36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="2:19" ht="15.75" customHeight="1">
@@ -4077,32 +4067,32 @@
       <c r="F46" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G46" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H46" s="46"/>
-      <c r="I46" s="47"/>
+      <c r="G46" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H46" s="52"/>
+      <c r="I46" s="53"/>
       <c r="J46" s="34" t="s">
         <v>2</v>
       </c>
       <c r="K46" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L46" s="10">
         <v>1</v>
       </c>
       <c r="M46" s="10"/>
       <c r="N46" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O46" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P46" s="42" t="s">
-        <v>250</v>
+        <v>234</v>
+      </c>
+      <c r="P46" s="41" t="s">
+        <v>247</v>
       </c>
       <c r="S46" s="36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="2:19" ht="15.75" customHeight="1">
@@ -4117,65 +4107,63 @@
       <c r="F47" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G47" s="50" t="s">
+      <c r="G47" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="H47" s="52"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="K47" s="35" t="s">
         <v>219</v>
-      </c>
-      <c r="H47" s="46"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="34" t="s">
-        <v>218</v>
-      </c>
-      <c r="K47" s="35" t="s">
-        <v>220</v>
       </c>
       <c r="L47" s="10">
         <v>1</v>
       </c>
       <c r="M47" s="10"/>
       <c r="N47" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O47" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P47" s="42" t="s">
-        <v>250</v>
+        <v>234</v>
+      </c>
+      <c r="P47" s="41" t="s">
+        <v>247</v>
       </c>
       <c r="S47" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="2:19" ht="15.75" customHeight="1">
-      <c r="B48" s="40" t="s">
-        <v>243</v>
-      </c>
+      <c r="B48" s="7"/>
       <c r="C48" s="8">
         <v>4</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="21"/>
       <c r="F48" s="11"/>
-      <c r="G48" s="66"/>
-      <c r="H48" s="46"/>
-      <c r="I48" s="47"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="53"/>
       <c r="J48" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K48" s="37" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="L48" s="10">
         <v>1</v>
       </c>
       <c r="M48" s="10"/>
       <c r="N48" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O48" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P48" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P48" s="41" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="15.75" customHeight="1">
@@ -4186,25 +4174,25 @@
       <c r="D49" s="9"/>
       <c r="E49" s="21"/>
       <c r="F49" s="11"/>
-      <c r="G49" s="66"/>
-      <c r="H49" s="46"/>
-      <c r="I49" s="47"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="53"/>
       <c r="J49" s="12"/>
       <c r="K49" s="37" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="L49" s="10">
         <v>1</v>
       </c>
       <c r="M49" s="10"/>
       <c r="N49" s="37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P49" s="42" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="P49" s="41" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="2:20" ht="15.75" customHeight="1">
@@ -4219,7 +4207,7 @@
       <c r="F50" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G50" s="45" t="s">
+      <c r="G50" s="47" t="s">
         <v>84</v>
       </c>
       <c r="H50" s="48"/>
@@ -4235,16 +4223,16 @@
       </c>
       <c r="M50" s="10"/>
       <c r="N50" s="31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O50" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P50" s="42" t="s">
-        <v>250</v>
+        <v>234</v>
+      </c>
+      <c r="P50" s="67" t="s">
+        <v>252</v>
       </c>
       <c r="S50" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="2:20" ht="15.75" customHeight="1">
@@ -4259,11 +4247,11 @@
       <c r="F51" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G51" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H51" s="46"/>
-      <c r="I51" s="47"/>
+      <c r="G51" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H51" s="52"/>
+      <c r="I51" s="53"/>
       <c r="J51" s="34" t="s">
         <v>2</v>
       </c>
@@ -4275,16 +4263,16 @@
       </c>
       <c r="M51" s="10"/>
       <c r="N51" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O51" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="P51" s="42" t="s">
-        <v>250</v>
+        <v>234</v>
+      </c>
+      <c r="P51" s="41" t="s">
+        <v>247</v>
       </c>
       <c r="S51" s="36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="2:20" ht="31.2">
@@ -4299,35 +4287,35 @@
       <c r="F52" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="G52" s="45" t="s">
+      <c r="G52" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="H52" s="46"/>
-      <c r="I52" s="47"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="53"/>
       <c r="J52" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K52" s="35" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="L52" s="10">
         <v>1</v>
       </c>
       <c r="M52" s="10"/>
       <c r="N52" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="O52" s="43" t="s">
-        <v>247</v>
-      </c>
-      <c r="P52" s="42" t="s">
-        <v>239</v>
-      </c>
-      <c r="S52" s="41" t="s">
-        <v>245</v>
+        <v>160</v>
+      </c>
+      <c r="O52" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="P52" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="S52" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="T52" s="39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="53" spans="2:20" ht="15.75" customHeight="1">
@@ -4342,32 +4330,32 @@
       <c r="F53" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="G53" s="45" t="s">
+      <c r="G53" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="46"/>
-      <c r="I53" s="47"/>
+      <c r="H53" s="52"/>
+      <c r="I53" s="53"/>
       <c r="J53" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K53" s="35" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="L53" s="10">
         <v>1</v>
       </c>
       <c r="M53" s="10"/>
       <c r="N53" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="O53" s="43" t="s">
-        <v>247</v>
-      </c>
-      <c r="P53" s="42" t="s">
-        <v>239</v>
+        <v>159</v>
+      </c>
+      <c r="O53" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="P53" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S53" s="36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="2:20" ht="15.75" customHeight="1">
@@ -4382,32 +4370,32 @@
       <c r="F54" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="G54" s="45" t="s">
+      <c r="G54" s="47" t="s">
         <v>81</v>
       </c>
       <c r="H54" s="48"/>
       <c r="I54" s="49"/>
       <c r="J54" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K54" s="35" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L54" s="10">
         <v>2</v>
       </c>
       <c r="M54" s="10"/>
       <c r="N54" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="O54" s="43" t="s">
-        <v>247</v>
-      </c>
-      <c r="P54" s="42" t="s">
-        <v>239</v>
+        <v>158</v>
+      </c>
+      <c r="O54" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="P54" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="S54" s="36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="2:20" ht="15.75" customHeight="1">
@@ -4416,9 +4404,9 @@
       <c r="D55" s="9"/>
       <c r="E55" s="21"/>
       <c r="F55" s="11"/>
-      <c r="G55" s="66"/>
-      <c r="H55" s="46"/>
-      <c r="I55" s="47"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="53"/>
       <c r="J55" s="12"/>
       <c r="K55" s="21"/>
       <c r="L55" s="10"/>
@@ -4433,9 +4421,9 @@
       <c r="D56" s="9"/>
       <c r="E56" s="21"/>
       <c r="F56" s="11"/>
-      <c r="G56" s="66"/>
-      <c r="H56" s="46"/>
-      <c r="I56" s="47"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="53"/>
       <c r="J56" s="12"/>
       <c r="K56" s="21"/>
       <c r="L56" s="10"/>
@@ -4450,9 +4438,9 @@
       <c r="D57" s="9"/>
       <c r="E57" s="21"/>
       <c r="F57" s="11"/>
-      <c r="G57" s="66"/>
-      <c r="H57" s="46"/>
-      <c r="I57" s="47"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="52"/>
+      <c r="I57" s="53"/>
       <c r="J57" s="12"/>
       <c r="K57" s="21"/>
       <c r="L57" s="10"/>
@@ -4467,9 +4455,9 @@
       <c r="D58" s="9"/>
       <c r="E58" s="21"/>
       <c r="F58" s="11"/>
-      <c r="G58" s="66"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="47"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="53"/>
       <c r="J58" s="12"/>
       <c r="K58" s="21"/>
       <c r="L58" s="10"/>
@@ -4484,7 +4472,7 @@
       <c r="D59" s="9"/>
       <c r="E59" s="21"/>
       <c r="F59" s="11"/>
-      <c r="G59" s="66"/>
+      <c r="G59" s="50"/>
       <c r="H59" s="48"/>
       <c r="I59" s="49"/>
       <c r="J59" s="12"/>
@@ -4501,6 +4489,61 @@
     <filterColumn colId="6" showButton="0"/>
   </autoFilter>
   <mergeCells count="71">
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:P2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G45:I45"/>
@@ -4517,61 +4560,6 @@
     <mergeCell ref="G58:I58"/>
     <mergeCell ref="G55:I55"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:P2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G40:I40"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <conditionalFormatting sqref="C7">

</xml_diff>